<commit_message>
te dhenat per kadaster done
</commit_message>
<xml_diff>
--- a/3-Katet/regjistri/29-Koordinatat-e-kateve-522-4-Softaj-Maliqi-leg.xlsx
+++ b/3-Katet/regjistri/29-Koordinatat-e-kateve-522-4-Softaj-Maliqi-leg.xlsx
@@ -1,36 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Softaj\ing\522-4-Softaj-Maliqi-leg\3-Katet\regjistri\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF871CE-4830-4729-822E-CBB8E0605D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="120" windowWidth="28395" windowHeight="15420"/>
+    <workbookView xWindow="540" yWindow="0" windowWidth="27795" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$60</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>Y</t>
   </si>
@@ -81,28 +79,25 @@
     <t>Terasa</t>
   </si>
   <si>
-    <t>PERDHESA</t>
-  </si>
-  <si>
     <t>Liridon Sejdiu</t>
   </si>
   <si>
-    <t>PERDHESA-TERAS</t>
+    <t>perdhese</t>
   </si>
   <si>
-    <t>PERDHESA-TERSA</t>
+    <t>Kati 1</t>
   </si>
   <si>
-    <t>BODRUMI</t>
+    <t>kati1</t>
   </si>
   <si>
-    <t>Bodrumi</t>
+    <t>kati1-terasa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,16 +431,16 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,8 +449,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -464,6 +458,39 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,7 +503,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -518,39 +545,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +583,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -644,7 +639,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E91F6037-E9CB-49EA-8E58-E0677C590B64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E91F6037-E9CB-49EA-8E58-E0677C590B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -705,7 +700,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07937452-2E79-4669-8F05-2069DFF859A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07937452-2E79-4669-8F05-2069DFF859A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -766,7 +761,7 @@
         <xdr:cNvPr id="6" name="TextBox 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD9F1684-A2E1-4EF0-89C9-1E368E9A0FDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD9F1684-A2E1-4EF0-89C9-1E368E9A0FDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -821,7 +816,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>: 00705-0</a:t>
+            <a:t>: 00522-4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -841,7 +836,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{87D2CC83-FE69-4C93-84EB-099D36DB81C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87D2CC83-FE69-4C93-84EB-099D36DB81C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1181,18 +1176,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,115 +1203,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="44"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1327,273 +1322,281 @@
       <c r="I12" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C15" s="5">
-        <v>4696954.0460000001</v>
+        <v>7516140.2470000004</v>
       </c>
       <c r="D15" s="5">
-        <v>7516707.0180000002</v>
+        <v>4695808.59</v>
       </c>
       <c r="E15" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="34">
-        <v>215.197</v>
+      <c r="I15" s="25">
+        <v>161.63</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5">
-        <v>4696948.3645000001</v>
+        <v>7516136.6969999997</v>
       </c>
       <c r="D16" s="5">
-        <v>7516704.6688000001</v>
+        <v>4695808.3540000003</v>
       </c>
       <c r="E16" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5">
-        <v>4696949.3219999997</v>
+        <v>7516135.8284999998</v>
       </c>
       <c r="D17" s="5">
-        <v>7516702.3550000004</v>
+        <v>4695807.6326000001</v>
       </c>
       <c r="E17" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5">
-        <v>4696943.1090000002</v>
+        <v>7516134.7712000003</v>
       </c>
       <c r="D18" s="5">
-        <v>7516699.7719999999</v>
+        <v>4695807.2357999999</v>
       </c>
       <c r="E18" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5">
-        <v>4696948.0159999998</v>
+        <v>7516133.8439999996</v>
       </c>
       <c r="D19" s="5">
-        <v>7516687.949</v>
+        <v>4695807.1710000001</v>
       </c>
       <c r="E19" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C20" s="5">
-        <v>4696952.3600000003</v>
+        <v>7516132.7161999997</v>
       </c>
       <c r="D20" s="5">
-        <v>7516689.7410000004</v>
+        <v>4695807.4112</v>
       </c>
       <c r="E20" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C21" s="5">
-        <v>4696953.9809999997</v>
+        <v>7516130.8260000004</v>
       </c>
       <c r="D21" s="5">
-        <v>7516685.8449999997</v>
+        <v>4695807.9331999999</v>
       </c>
       <c r="E21" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C22" s="5">
-        <v>4696961.5599999996</v>
+        <v>7516129.8949999996</v>
       </c>
       <c r="D22" s="5">
-        <v>7516688.9299999997</v>
+        <v>4695821.3059999999</v>
       </c>
       <c r="E22" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="C23" s="5">
-        <v>4696948.3389999997</v>
+        <v>7516143.4210000001</v>
       </c>
       <c r="D23" s="5">
-        <v>7516705.3679999998</v>
+        <v>4695813.0669999998</v>
       </c>
       <c r="E23" s="10">
-        <v>615.05600000000004</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="C24" s="5">
-        <v>4696943.0360000003</v>
+        <v>7516142.7883000001</v>
       </c>
       <c r="D24" s="5">
-        <v>7516703.1349999998</v>
+        <v>4695822.1886</v>
       </c>
       <c r="E24" s="10">
-        <v>615.05200000000002</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="10">
-        <v>17.486000000000001</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="C25" s="5">
-        <v>4696944.2389000002</v>
+        <v>7516139.9567</v>
       </c>
       <c r="D25" s="5">
-        <v>7516700.2417000001</v>
+        <v>4695812.8307999996</v>
       </c>
       <c r="E25" s="10">
-        <v>615.04899999999998</v>
+        <v>616.65899999999999</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="25"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>130</v>
+      </c>
+      <c r="C26" s="5">
+        <v>7516131.7905000001</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4695807.9702000003</v>
+      </c>
+      <c r="E26" s="10">
+        <v>616.65899999999999</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="15">
-        <f>SUM(I15:I24)</f>
-        <v>232.68299999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="I26" s="14">
+        <f>SUM(I15:I25)</f>
+        <v>161.63</v>
+      </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D27" s="6"/>
@@ -1604,265 +1607,353 @@
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G29" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I29" s="13" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="11">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5">
-        <v>4696955.0115999999</v>
-      </c>
-      <c r="D29" s="5">
-        <v>7516704.6935000001</v>
-      </c>
-      <c r="E29" s="10">
-        <v>612.553</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="34">
-        <v>170.02</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C30" s="5">
-        <v>4696948.3645000001</v>
+        <v>7516129.8949999996</v>
       </c>
       <c r="D30" s="5">
-        <v>7516704.6688000001</v>
+        <v>4695821.3059999999</v>
       </c>
       <c r="E30" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="44">
+        <v>118.154</v>
+      </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C31" s="5">
-        <v>4696949.3219999997</v>
+        <v>7516142.7883000001</v>
       </c>
       <c r="D31" s="5">
-        <v>7516702.3550000004</v>
+        <v>4695822.1886</v>
       </c>
       <c r="E31" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="G31" s="25"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C32" s="5">
-        <v>4696943.1090000002</v>
+        <v>7516130.5286999997</v>
       </c>
       <c r="D32" s="5">
-        <v>7516699.7719999999</v>
+        <v>4695812.1853999998</v>
       </c>
       <c r="E32" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="G32" s="25"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="C33" s="5">
-        <v>4696948.0159999998</v>
+        <v>7516143.4220000003</v>
       </c>
       <c r="D33" s="5">
-        <v>7516687.949</v>
+        <v>4695813.068</v>
       </c>
       <c r="E33" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="G33" s="25"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C34" s="5">
-        <v>4696959.9238999998</v>
+        <v>7516140.3609999996</v>
       </c>
       <c r="D34" s="5">
-        <v>7516692.8684999999</v>
+        <v>4695807.8439999996</v>
       </c>
       <c r="E34" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="10">
+        <v>46.505000000000003</v>
+      </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C35" s="5">
-        <v>4696950.2127</v>
+        <v>7516137.2699999996</v>
       </c>
       <c r="D35" s="5">
-        <v>7516705.4330000002</v>
+        <v>4695807.6560000004</v>
       </c>
       <c r="E35" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="34"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C36" s="5">
-        <v>4696951.1744999997</v>
+        <v>7516137.2230000002</v>
       </c>
       <c r="D36" s="5">
-        <v>7516703.1069</v>
+        <v>4695808.2949999999</v>
       </c>
       <c r="E36" s="10">
-        <v>612.553</v>
+        <v>619.90599999999995</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="15" t="s">
+      <c r="G36" s="25"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="11">
+        <v>85</v>
+      </c>
+      <c r="C37" s="5">
+        <v>7516136.7510000002</v>
+      </c>
+      <c r="D37" s="5">
+        <v>4695808.2759999996</v>
+      </c>
+      <c r="E37" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="25"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <v>86</v>
+      </c>
+      <c r="C38" s="5">
+        <v>7516135.858</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4695807.58</v>
+      </c>
+      <c r="E38" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="25"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <v>87</v>
+      </c>
+      <c r="C39" s="5">
+        <v>7516134.784</v>
+      </c>
+      <c r="D39" s="5">
+        <v>4695807.1770000001</v>
+      </c>
+      <c r="E39" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="25"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <v>88</v>
+      </c>
+      <c r="C40" s="5">
+        <v>7516133.8439999996</v>
+      </c>
+      <c r="D40" s="5">
+        <v>4695807.1109999996</v>
+      </c>
+      <c r="E40" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="25"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="11">
+        <v>89</v>
+      </c>
+      <c r="C41" s="5">
+        <v>7516132.6940000001</v>
+      </c>
+      <c r="D41" s="5">
+        <v>4695807.3550000004</v>
+      </c>
+      <c r="E41" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>90</v>
+      </c>
+      <c r="C42" s="5">
+        <v>7516131.7750000004</v>
+      </c>
+      <c r="D42" s="5">
+        <v>4695807.91</v>
+      </c>
+      <c r="E42" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="25"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="11">
+        <v>91</v>
+      </c>
+      <c r="C43" s="5">
+        <v>7516130.8283000002</v>
+      </c>
+      <c r="D43" s="5">
+        <v>4695807.8737000003</v>
+      </c>
+      <c r="E43" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="25"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <v>92</v>
+      </c>
+      <c r="C44" s="5">
+        <v>7516140.0192999998</v>
+      </c>
+      <c r="D44" s="5">
+        <v>4695812.8350999998</v>
+      </c>
+      <c r="E44" s="10">
+        <v>619.90599999999995</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="H44" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="15">
-        <f>SUM(I29:I35)</f>
-        <v>170.02</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="I44" s="14">
+        <f>SUM(I30:I34)</f>
+        <v>164.65899999999999</v>
+      </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D45" s="6"/>
@@ -1897,79 +1988,139 @@
       <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K50" s="1"/>
-    </row>
-    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+    </row>
+    <row r="58" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="26"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="21" t="s">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" s="36"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I51" s="22"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="17"/>
-    </row>
-    <row r="52" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="28" t="s">
+      <c r="I59" s="32"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="27"/>
+    </row>
+    <row r="60" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="31">
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41">
         <v>140</v>
       </c>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="19"/>
-    </row>
-    <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K55" s="1"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="29"/>
+    </row>
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K63" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="12">
+    <mergeCell ref="J59:K60"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="G30:G44"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="C8:J10"/>
-    <mergeCell ref="G15:G25"/>
-    <mergeCell ref="H15:H23"/>
-    <mergeCell ref="I15:I23"/>
-    <mergeCell ref="J51:K52"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H51:I52"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="G29:G36"/>
-    <mergeCell ref="H29:H34"/>
-    <mergeCell ref="I29:I34"/>
+    <mergeCell ref="G15:G26"/>
+    <mergeCell ref="H15:H24"/>
+    <mergeCell ref="I15:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>